<commit_message>
Update the planning folder with todays minutes and new wireframe
</commit_message>
<xml_diff>
--- a/Planning/Spice Girls/Resources_References.xlsx
+++ b/Planning/Spice Girls/Resources_References.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="API" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="References Publications" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Summary Description" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,23 +13,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>API Page</t>
   </si>
   <si>
-    <t>https://spoonacular.com/food-api</t>
-  </si>
-  <si>
-    <t>https://api.spoonacular.com/recipes/716429/information?apiKey=c5413da4ad594941bce9e89fdadec43c&amp;includeNutrition=true</t>
-  </si>
-  <si>
-    <t>https://www.programmableweb.com/category/food/apis?category=20048</t>
-  </si>
-  <si>
-    <t>http://www.recipepuppy.com/api/?i=onions,garlic&amp;q=omelet&amp;p=3</t>
-  </si>
-  <si>
     <t>https://developer.edamam.com/edamam-docs-recipe-api</t>
   </si>
   <si>
@@ -36,39 +25,6 @@
   </si>
   <si>
     <t>app_key=819a5992ef814566f4860aaaf9edec40</t>
-  </si>
-  <si>
-    <t>Components:</t>
-  </si>
-  <si>
-    <t>Nav Bar - Hamburger menu/Logo</t>
-  </si>
-  <si>
-    <t>Home Page Gallery</t>
-  </si>
-  <si>
-    <t>Recipe Page</t>
-  </si>
-  <si>
-    <t>Contact Page/About Us</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Features:</t>
-  </si>
-  <si>
-    <t>Add Comment</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>Nav within Recipe page</t>
   </si>
   <si>
     <t xml:space="preserve">References: </t>
@@ -88,12 +44,36 @@
   <si>
     <t>Tai, Grace. 2020. Cooking Recipe App Design. URL: http://www.gracetai.com/portfolio/cooking-recipe-app-design/ . Date Accessed: July 31, 2020</t>
   </si>
+  <si>
+    <t>Recipe Label</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>URL:</t>
+  </si>
+  <si>
+    <t>Chicken Vesuvio Recipe</t>
+  </si>
+  <si>
+    <t>Though it's not an authentic Italian dish, Chicken Vesuvio
+ tastes like it could be. In actuality, it's a specialty of the 
+Italian-American restaurants in my home town of Chicago, invented 
+sometime in the 1930s and still going strong as a favorite around town. 
+ It's a rich, stewed dish with key elements of creamy potatoes, white 
+wine, and plenty of garlic—as well as the final sprinkle of peas to give
+ it color and freshness. - Serious Eats, 2019</t>
+  </si>
+  <si>
+    <t>https://www.seriouseats.com/recipes/2011/12/chicken-vesuvio-recipe.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -105,16 +85,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <u/>
       <color rgb="FF0000FF"/>
     </font>
     <font/>
@@ -123,18 +93,12 @@
       <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -153,17 +117,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -179,6 +136,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -395,104 +356,18 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -508,17 +383,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
+      <c r="A2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -527,4 +402,48 @@
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.43"/>
+    <col customWidth="1" min="2" max="2" width="62.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>